<commit_message>
CSmatchSht added optional parameter
</commit_message>
<xml_diff>
--- a/match2.0/match_environment.xlsx
+++ b/match2.0/match_environment.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="-15" yWindow="-15" windowWidth="8880" windowHeight="10080"/>
+    <workbookView xWindow="-12" yWindow="-12" windowWidth="8880" windowHeight="10080"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -22,9 +22,6 @@
   </si>
   <si>
     <t>Pavel Khrapkin</t>
-  </si>
-  <si>
-    <t>C:\Users\Pavel_Khrapkin\Documents\Pavel\match\Match2.0\DBs\</t>
   </si>
   <si>
     <r>
@@ -41,6 +38,9 @@
       </rPr>
       <t>C:\match_environment.xlsx</t>
     </r>
+  </si>
+  <si>
+    <t>C:\DBs\</t>
   </si>
 </sst>
 </file>
@@ -124,7 +124,7 @@
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Обычный" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -137,9 +137,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Тема Office">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Стандартная">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -177,7 +177,7 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Стандартная">
       <a:majorFont>
         <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
@@ -249,7 +249,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Стандартная">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -427,33 +427,33 @@
   <dimension ref="A1:B3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="28.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="28.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="1">
         <v>41176.731400462966</v>
       </c>
       <c r="B1" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="B2" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
   </sheetData>
@@ -468,7 +468,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -481,7 +481,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>